<commit_message>
SNCE, UNH, other changes
</commit_message>
<xml_diff>
--- a/HC Services.xlsx
+++ b/HC Services.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\CODE\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3167E7-0A2C-43CB-A6D1-3918FD700AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA9C298-3702-4D51-A222-01962C3A16B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="510" windowWidth="20310" windowHeight="14910" xr2:uid="{C4E93C08-663D-492A-AEC7-938C289047C3}"/>
+    <workbookView xWindow="5940" yWindow="2205" windowWidth="31035" windowHeight="17985" xr2:uid="{C4E93C08-663D-492A-AEC7-938C289047C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Private" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -167,16 +171,53 @@
   </si>
   <si>
     <t>300015 CH</t>
+  </si>
+  <si>
+    <t>Science 37</t>
+  </si>
+  <si>
+    <t>SNCE</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Syapse</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Q222</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -198,13 +239,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -218,6 +274,37 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Models"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="N3">
+            <v>116.348405</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="N5">
+            <v>148.32900000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -517,43 +604,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F7AEE9-EF00-4FDA-B370-F11DB8E9EFA2}">
-  <dimension ref="B2:E23"/>
+  <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="10" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="5">
+        <v>544.70000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -561,7 +668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -569,7 +676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -577,7 +684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -585,7 +692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -593,7 +700,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -601,7 +708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -609,7 +716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -617,7 +724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -625,7 +732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -633,7 +740,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>24</v>
       </c>
@@ -641,7 +748,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -649,7 +756,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>28</v>
       </c>
@@ -657,7 +764,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>30</v>
       </c>
@@ -665,7 +772,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -673,7 +780,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -681,7 +788,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>36</v>
       </c>
@@ -689,7 +796,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -697,7 +804,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>40</v>
       </c>
@@ -705,7 +812,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>42</v>
       </c>
@@ -713,7 +820,72 @@
         <v>43</v>
       </c>
     </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.79</v>
+      </c>
+      <c r="E24" s="3">
+        <f>+[1]Main!$N$3</f>
+        <v>116.348405</v>
+      </c>
+      <c r="F24" s="3">
+        <f>+D24*E24</f>
+        <v>208.26364495000001</v>
+      </c>
+      <c r="G24" s="3">
+        <f>+[1]Main!$N$5-[1]Main!$N$6</f>
+        <v>148.32900000000001</v>
+      </c>
+      <c r="H24" s="3">
+        <f>+F24-G24</f>
+        <v>59.934644950000006</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="4">
+        <v>44791</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B24" r:id="rId1" xr:uid="{D0C0A315-E060-4161-8384-69E332154276}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DE9255-CFE9-4043-A2BC-99E9D42B4CC5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Main!A1" display="Main" xr:uid="{A0D2358C-D33C-4497-9BB4-74B0882B5080}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>